<commit_message>
uploading new successful list
</commit_message>
<xml_diff>
--- a/public/template/interview_status.xlsx
+++ b/public/template/interview_status.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yusufolatunji/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yusufolatunji/MyProject/Web/dcssportal/public/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D3CCFB0-C1BB-8B48-B85A-5E71E91A1C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A5FA92-1949-964B-B4EC-02842B4CA45B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15700" xr2:uid="{B95154BD-71C2-E744-A289-76DD3791276D}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15620" xr2:uid="{B95154BD-71C2-E744-A289-76DD3791276D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>exam_number</t>
+  </si>
+  <si>
+    <t>score</t>
   </si>
 </sst>
 </file>
@@ -410,7 +413,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEAA6F0C-E803-4242-BABD-79E2D9DB3623}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -421,9 +424,12 @@
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>